<commit_message>
Changed default max workers to 10, Added auto retry on failure for a thread, Added error logging
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,39 +458,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wood, B. Dan, and Richard W. Waterman. “The Dynamics of Political Control of the Bureaucracy.” American Political Science Review 85, no. 3 (1991): 801–28. https://doi.org/10.2307/1963851.</t>
+          <t>Paris, David C. “Moral Education and the ‘Tie That Binds’ in Liberal Political Theory.” American Political Science Review 85, no. 3 (1991): 875–901. https://doi.org/10.2307/1963854.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A new paradigm of political-bureaucratic relations emerged through the 1980s holding that U.S. democratic institutions continuously shape nonelective public bureaucracies. Several empirical studies support the paradigm with evidence suggestive of political manipulation but none reveals the scope or specific mechanisms of political control. We explore the dynamics of political control of the bureaucracy explicitly to determine the scope and mechanisms. We examine output time series from seven different public bureaucracies for responsiveness to political tools applied in the late Carter and early Reagan administrations. We find responsiveness in all seven cases. The evidence also shows that political appointments—a shared power of the president and Congress—is the most important instrument of political control; changing budgets, legislation, congressional signals, and administrative reorganizations are less important. These findings confirm intuitive assertions by institutional scholars and suggest a method of “policy monitoring” that could enhance future democratic control of the bureaucracy.</t>
+          <t>I examine the search for a “tie that binds, “ or “core” values, in liberal political theory, specifically Rawls's recent arguments, and in proposals concerning moral education in the public schools. Both Rawls and the proponents of moral education appeal to consensus or shared values, but the search for core values in both theory and practice is only partly successful. Specifically, this search is misguided insofar as it does not reflect how values are embedded in specific institutions and practices. The various forms of moral education in the public schools, both implicit and explicit, illustrate a consensus about a range of moral and intellectual virtues that is broader and more complex than arguments for core values allow. Comparing arguments concerning core values in political theory and moral education suggests how liberal political theory might deal with questions of consensus, justification, and the task of political theory generally.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Texas A&amp;M University</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>University of New Mexico</t>
-        </is>
-      </c>
+          <t>Hamilton College</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Remmer, Karen L. “The Political Impact of Economic Crisis in Latin America in the 1980s.” American Political Science Review 85, no. 3 (1991): 777–800. https://doi.org/10.2307/1963850.</t>
+          <t>Richardson, Bradley M. “European Party Loyalties Revisited.” American Political Science Review 85, no. 3 (1991): 751–75. https://doi.org/10.2307/1963849.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Research on the political implications of economic conditions is separated into two relatively distinct bodies of literature. I bridge the theoretical gap between them by examining the effects of economic crisis on electoral outcomes in Latin America from 1982 to 1990. An analysis of 21 competitive elections indicates that crisis conditions undermine support for incumbents and provoke high levels of electoral volatility but without necessarily fostering the growth of political extremism or the exhaustion of elite consensus associated with the breakdown of democracy. The results also suggest that the relationship between economic conditions and electoral instability is mediated by party system structure rather than democratic age. Paradoxically, the findings buttress prior research on electoral outcomes in the comparatively stable and homogeneous Organization for Economic Cooperation and Development (OECD) nations while undercutting theoretical frameworks elaborated with specific reference to the breakdown and consolidation of Third World democracy.</t>
+          <t>The likelihood that party loyalties reflect the characteristics of parties and political competition within specific political environments was generally ignored in critiques of party identification abroad. In this article, I identify substantial frequencies of stable partisan ties among British, Dutch, and German voters in the 1960s through the 1980s. Stable party loyalists in turn usually vote for their preferred party in subsequent elections. Long-term partisan ties are most common among supporters of traditional cleavage parties. These long-term party loyalties reflect the effects of both long-standing hostilities toward opposing parties and well-developed party principles. Since partisan responses are internally consistent and subsume ideational as well as affective components, these feelings resemble social psychology's affect-laden schemata.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>University of New Mexico</t>
+          <t>Ohio State University</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -516,100 +512,104 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Richardson, Bradley M. “European Party Loyalties Revisited.” American Political Science Review 85, no. 3 (1991): 751–75. https://doi.org/10.2307/1963849.</t>
+          <t>Quinn, Dennis P., and Robert Y. Shapiro. “Business Political Power: The Case of Taxation.” American Political Science Review 85, no. 3 (1991): 851–74. https://doi.org/10.2307/1963853.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>The likelihood that party loyalties reflect the characteristics of parties and political competition within specific political environments was generally ignored in critiques of party identification abroad. In this article, I identify substantial frequencies of stable partisan ties among British, Dutch, and German voters in the 1960s through the 1980s. Stable party loyalists in turn usually vote for their preferred party in subsequent elections. Long-term partisan ties are most common among supporters of traditional cleavage parties. These long-term party loyalties reflect the effects of both long-standing hostilities toward opposing parties and well-developed party principles. Since partisan responses are internally consistent and subsume ideational as well as affective components, these feelings resemble social psychology's affect-laden schemata.</t>
+          <t>We examine contending views about the forms and mechanisms of business power in U.S. politics by estimating time series models explaining taxation and redistribution. Taxation and redistribution constitute strong cases for theories about business and class power, since all firms have an interest in reducing taxation. We find that changes in corporate taxation and in redistribution between capital gains income and earned income and between corporate taxation and individual taxation are strongly influenced by political partisanship, with Democratic administrations increasing the tax burden on firms and their owners. How far corporations engage in electoral financing—measured through the establishment of corporate political action committees—is also influential. The models show some evidence consistent with the understanding of class power conceptualized by Bowles, Gordon, and Weisskopf and the presence of election cycle effects but inconsistent with implications arising from the structural dependence of the state on capital and asset concentration in the largest corporations as a mechanism of class power.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ohio State University</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>Georgetown University</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Columbia University</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Snidal, Duncan. “Relative Gains and the Pattern of International Cooperation.” American Political Science Review 85, no. 3 (1991): 701–26. https://doi.org/10.2307/1963847.</t>
+          <t>Scholz, John T., Jim Twombly, and Barbara Headrick. “Street-Level Political Controls Over Federal Bureaucracy.” American Political Science Review 85, no. 3 (1991): 829–50. https://doi.org/10.2307/1963852.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Many political situations involve competitions where winning is more important than doing well. In international politics, this relative gains problem is widely argued to be a major impediment to cooperation under anarchy. After discussing why states might seek relative gains, I demonstrate that the hypothesis holds very different implications from those usually presumed. Relative gains do impede cooperation in the two-actor case and provide an important justification for treating international anarchy as a prisoner's dilemma problem; but if the initial absolute gains situation is not a prisoner's dilemma, relative gains seeking is much less consequential. Its significance is even more attenuated with more than two competitors. Relative gains cannot prop up the realist critique of international cooperation theory, but may affect the pattern of cooperation when a small number of states are the most central international actors.</t>
+          <t>Local partisan activities of legislators and their electoral coalitions systematically influence field office activities of federal bureaucracies in their electoral districts. This alternative to centralized democratic controls over bureaucracy occurs because discretionary policy decisions made at the field office level are influenced by local resources generated through partisan activities. Our study of county-level Occupational Safety and Health Administration enforcement in New York (1976–85) finds that county, state, and federal elected officials influence local enforcement activities, with liberal, Democratic legislators associated with more active enforcement. The county political parties are most influential for activities with the most local discretion, while members of Congress are more influential for local activities more readily controlled by the national office.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>University of Chicago</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+          <t>State University of New York Stony Brook</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>State University of New York Buffalo / Texas A&amp;M University</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Scholz, John T., Jim Twombly, and Barbara Headrick. “Street-Level Political Controls Over Federal Bureaucracy.” American Political Science Review 85, no. 3 (1991): 829–50. https://doi.org/10.2307/1963852.</t>
+          <t>Snidal, Duncan. “Relative Gains and the Pattern of International Cooperation.” American Political Science Review 85, no. 3 (1991): 701–26. https://doi.org/10.2307/1963847.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Local partisan activities of legislators and their electoral coalitions systematically influence field office activities of federal bureaucracies in their electoral districts. This alternative to centralized democratic controls over bureaucracy occurs because discretionary policy decisions made at the field office level are influenced by local resources generated through partisan activities. Our study of county-level Occupational Safety and Health Administration enforcement in New York (1976–85) finds that county, state, and federal elected officials influence local enforcement activities, with liberal, Democratic legislators associated with more active enforcement. The county political parties are most influential for activities with the most local discretion, while members of Congress are more influential for local activities more readily controlled by the national office.</t>
+          <t>Many political situations involve competitions where winning is more important than doing well. In international politics, this relative gains problem is widely argued to be a major impediment to cooperation under anarchy. After discussing why states might seek relative gains, I demonstrate that the hypothesis holds very different implications from those usually presumed. Relative gains do impede cooperation in the two-actor case and provide an important justification for treating international anarchy as a prisoner's dilemma problem; but if the initial absolute gains situation is not a prisoner's dilemma, relative gains seeking is much less consequential. Its significance is even more attenuated with more than two competitors. Relative gains cannot prop up the realist critique of international cooperation theory, but may affect the pattern of cooperation when a small number of states are the most central international actors.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>State University of New York Stony Brook</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>State University of New York Buffalo / Texas A&amp;M University</t>
-        </is>
-      </c>
+          <t>University of Chicago</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Quinn, Dennis P., and Robert Y. Shapiro. “Business Political Power: The Case of Taxation.” American Political Science Review 85, no. 3 (1991): 851–74. https://doi.org/10.2307/1963853.</t>
+          <t>Remmer, Karen L. “The Political Impact of Economic Crisis in Latin America in the 1980s.” American Political Science Review 85, no. 3 (1991): 777–800. https://doi.org/10.2307/1963850.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>We examine contending views about the forms and mechanisms of business power in U.S. politics by estimating time series models explaining taxation and redistribution. Taxation and redistribution constitute strong cases for theories about business and class power, since all firms have an interest in reducing taxation. We find that changes in corporate taxation and in redistribution between capital gains income and earned income and between corporate taxation and individual taxation are strongly influenced by political partisanship, with Democratic administrations increasing the tax burden on firms and their owners. How far corporations engage in electoral financing—measured through the establishment of corporate political action committees—is also influential. The models show some evidence consistent with the understanding of class power conceptualized by Bowles, Gordon, and Weisskopf and the presence of election cycle effects but inconsistent with implications arising from the structural dependence of the state on capital and asset concentration in the largest corporations as a mechanism of class power.</t>
+          <t>Research on the political implications of economic conditions is separated into two relatively distinct bodies of literature. I bridge the theoretical gap between them by examining the effects of economic crisis on electoral outcomes in Latin America from 1982 to 1990. An analysis of 21 competitive elections indicates that crisis conditions undermine support for incumbents and provoke high levels of electoral volatility but without necessarily fostering the growth of political extremism or the exhaustion of elite consensus associated with the breakdown of democracy. The results also suggest that the relationship between economic conditions and electoral instability is mediated by party system structure rather than democratic age. Paradoxically, the findings buttress prior research on electoral outcomes in the comparatively stable and homogeneous Organization for Economic Cooperation and Development (OECD) nations while undercutting theoretical frameworks elaborated with specific reference to the breakdown and consolidation of Third World democracy.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Georgetown University</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Columbia University</t>
-        </is>
-      </c>
+          <t>University of New Mexico</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Paris, David C. “Moral Education and the ‘Tie That Binds’ in Liberal Political Theory.” American Political Science Review 85, no. 3 (1991): 875–901. https://doi.org/10.2307/1963854.</t>
+          <t>Wood, B. Dan, and Richard W. Waterman. “The Dynamics of Political Control of the Bureaucracy.” American Political Science Review 85, no. 3 (1991): 801–28. https://doi.org/10.2307/1963851.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>I examine the search for a “tie that binds, “ or “core” values, in liberal political theory, specifically Rawls's recent arguments, and in proposals concerning moral education in the public schools. Both Rawls and the proponents of moral education appeal to consensus or shared values, but the search for core values in both theory and practice is only partly successful. Specifically, this search is misguided insofar as it does not reflect how values are embedded in specific institutions and practices. The various forms of moral education in the public schools, both implicit and explicit, illustrate a consensus about a range of moral and intellectual virtues that is broader and more complex than arguments for core values allow. Comparing arguments concerning core values in political theory and moral education suggests how liberal political theory might deal with questions of consensus, justification, and the task of political theory generally.</t>
+          <t>A new paradigm of political-bureaucratic relations emerged through the 1980s holding that U.S. democratic institutions continuously shape nonelective public bureaucracies. Several empirical studies support the paradigm with evidence suggestive of political manipulation but none reveals the scope or specific mechanisms of political control. We explore the dynamics of political control of the bureaucracy explicitly to determine the scope and mechanisms. We examine output time series from seven different public bureaucracies for responsiveness to political tools applied in the late Carter and early Reagan administrations. We find responsiveness in all seven cases. The evidence also shows that political appointments—a shared power of the president and Congress—is the most important instrument of political control; changing budgets, legislation, congressional signals, and administrative reorganizations are less important. These findings confirm intuitive assertions by institutional scholars and suggest a method of “policy monitoring” that could enhance future democratic control of the bureaucracy.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hamilton College</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
+          <t>Texas A&amp;M University</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>University of New Mexico</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Scrape all pages and include everything except book review and front/back matter
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,115 +458,125 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Paris, David C. “Moral Education and the ‘Tie That Binds’ in Liberal Political Theory.” American Political Science Review 85, no. 3 (1991): 875–901. https://doi.org/10.2307/1963854.</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>I examine the search for a “tie that binds, “ or “core” values, in liberal political theory, specifically Rawls's recent arguments, and in proposals concerning moral education in the public schools. Both Rawls and the proponents of moral education appeal to consensus or shared values, but the search for core values in both theory and practice is only partly successful. Specifically, this search is misguided insofar as it does not reflect how values are embedded in specific institutions and practices. The various forms of moral education in the public schools, both implicit and explicit, illustrate a consensus about a range of moral and intellectual virtues that is broader and more complex than arguments for core values allow. Comparing arguments concerning core values in political theory and moral education suggests how liberal political theory might deal with questions of consensus, justification, and the task of political theory generally.</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Hamilton College</t>
-        </is>
-      </c>
+          <t>“Erratum.” American Political Science Review 85, no. 1 (1991): 234–234. https://doi.org/10.2307/1962964.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Richardson, Bradley M. “European Party Loyalties Revisited.” American Political Science Review 85, no. 3 (1991): 751–75. https://doi.org/10.2307/1963849.</t>
+          <t>Abramson, Paul R., and Charles W. Ostrom. “Macropartisanship: An Empirical Reassessment.” American Political Science Review 85, no. 1 (1991): 181–92. https://doi.org/10.2307/1962884.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The likelihood that party loyalties reflect the characteristics of parties and political competition within specific political environments was generally ignored in critiques of party identification abroad. In this article, I identify substantial frequencies of stable partisan ties among British, Dutch, and German voters in the 1960s through the 1980s. Stable party loyalists in turn usually vote for their preferred party in subsequent elections. Long-term partisan ties are most common among supporters of traditional cleavage parties. These long-term party loyalties reflect the effects of both long-standing hostilities toward opposing parties and well-developed party principles. Since partisan responses are internally consistent and subsume ideational as well as affective components, these feelings resemble social psychology's affect-laden schemata.</t>
+          <t>To evaluate the comparability of the Gallup and Michigan Survey Research Center measures for studying levels of partisanship among the U.S. electorate we compare the overtime distribution of partisanship and the correlates of partisanship using the results of Gallup surveys, the National Election Studies, and the General Social Surveys. Compared with the Gallup results, both the other two surveys reveal less short-term variation and also less total variation. Compared with the Gallup results, the National Election Studies partisanship results are less related to short-term electoral outcomes and do not appear to be strongly driven by short-term economic and political evaluations. Our analyses suggest that scholars should be cautious about using Gallup results to revise conclusions based upon analyses that employ the Michigan Survey Research Center party identification measure.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ohio State University</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+          <t>Michigan State University</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Michigan State University</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Wagner, R. Harrison. “Nuclear Deterrence, Counterforce Strategies, and the Incentive to Strike First.” American Political Science Review 85, no. 3 (1991): 727–49. https://doi.org/10.2307/1963848.</t>
+          <t>Rapoport, Ronald B., Walter J. Stone, and Alan I. Abramowitz. “Do Endorsements Matter? Group Influence in the 1984 Democratic Caucuses.” American Political Science Review 85, no. 1 (1991): 193–203. https://doi.org/10.2307/1962885.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I use the theory of games to investigate issues about how to understand the use of nuclear counterforce strategies by the United States and the Soviet Union during the Cold War. The function of the counterforce strategies I model is not to enable a state confidently to launch a nuclear attack but to convince its adversary that the probability that it might do so as a last resort is greater than zero. The models allow one to investigate rational behavior when information is incomplete and there is an incentive to strike first, and therefore provide a way to explore controversies about the effect of counterforce strategies on both the credibility of extended deterrence and the possibility of inadvertent nuclear war. The models suggest, contrary to the claims of a number of writers, that the use of nuclear counterforce strategies is not necessarily inconsistent with rational behavior and provide some insight into the relation between counterforce strategies and brinkmanship models of deterrence.</t>
+          <t>Although candidates are very concerned about garnering prenomination group endorsements, there is virtually no research on the effects of such endorsements at the presidential level. In 1984, teachers', women's, and labor groups all endorsed Mondale for the Democratic nomination. Using a survey of Democratic caucus participants, we examine the effects of these endorsements on both candidate support and prenomination activity for the endorsed candidate. We find substantial effects of labor and teachers' group endorsements on the candidate choice of their members, but virtually no effect of women's groups. Labor union membership also had the greatest impact on campaign activity for Mondale.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>University of Texas Austin</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>College of William and Mary</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>University of Colorado / Emory University</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Quinn, Dennis P., and Robert Y. Shapiro. “Business Political Power: The Case of Taxation.” American Political Science Review 85, no. 3 (1991): 851–74. https://doi.org/10.2307/1963853.</t>
+          <t>Scholz, John T. “Cooperative Regulatory Enforcement and the Politics of Administrative Effectiveness.” American Political Science Review 85, no. 1 (1991): 115–36. https://doi.org/10.2307/1962881.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>We examine contending views about the forms and mechanisms of business power in U.S. politics by estimating time series models explaining taxation and redistribution. Taxation and redistribution constitute strong cases for theories about business and class power, since all firms have an interest in reducing taxation. We find that changes in corporate taxation and in redistribution between capital gains income and earned income and between corporate taxation and individual taxation are strongly influenced by political partisanship, with Democratic administrations increasing the tax burden on firms and their owners. How far corporations engage in electoral financing—measured through the establishment of corporate political action committees—is also influential. The models show some evidence consistent with the understanding of class power conceptualized by Bowles, Gordon, and Weisskopf and the presence of election cycle effects but inconsistent with implications arising from the structural dependence of the state on capital and asset concentration in the largest corporations as a mechanism of class power.</t>
+          <t>Even when political interests control bureaucratic outputs, the control of policy outcomes is complicated by trade-offs between controllable versus effective implementation strategies. I use a nested game framework to explain why a cooperative strategy can increase enforcement effectiveness in the narrow administrative game and why principal-agent control problems and collective action problems associated with the strategy lead policy beneficiaries to oppose the effective strategy in the broader political games. Analyses of state-level Occupational Safety and Health Administration enforcement provide evidence that cooperation does enhance the impact of enforcement in reducing workplace injury rates but that policy beneficiaries oppose and sabotage cooperation. The interactions between administrative effectiveness and interest group politics in this and other implementation situations require that both be analyzed simultaneously, and the nested game framework can provide a systematic approach to such analyses.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Georgetown University</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Columbia University</t>
-        </is>
-      </c>
+          <t>State University of New York Stony Brook</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Scholz, John T., Jim Twombly, and Barbara Headrick. “Street-Level Political Controls Over Federal Bureaucracy.” American Political Science Review 85, no. 3 (1991): 829–50. https://doi.org/10.2307/1963852.</t>
+          <t>Cohen, Jeffrey E., Michael A. Krassa, and John A. Hamman. “The Impact of Presidential Campaigning on Midterm U.S. Senate Elections.” American Political Science Review 85, no. 1 (1991): 165–78. https://doi.org/10.2307/1962883.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Local partisan activities of legislators and their electoral coalitions systematically influence field office activities of federal bureaucracies in their electoral districts. This alternative to centralized democratic controls over bureaucracy occurs because discretionary policy decisions made at the field office level are influenced by local resources generated through partisan activities. Our study of county-level Occupational Safety and Health Administration enforcement in New York (1976–85) finds that county, state, and federal elected officials influence local enforcement activities, with liberal, Democratic legislators associated with more active enforcement. The county political parties are most influential for activities with the most local discretion, while members of Congress are more influential for local activities more readily controlled by the national office.</t>
+          <t>The conventional wisdom about presidential campaigning in midterm Senate elections is that presidential efforts lack impact or have negative impact. We discuss conceptual problems with the conventional view and offer an alternative that views presidential campaigning as strategic. We test this alternative and find support for it. Further, we find that presidential campaign efforts have a positive impact on the vote through the mobilization of nonvoters. Finally, in a significant number of cases, presidential campaigning may have been the margin of victory for candidates of the president's party. We discuss the implications of these findings on assessments of the president and relations with Congress during the second half of the term.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>State University of New York Stony Brook</t>
+          <t>University of Illinois Urbana</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>State University of New York Buffalo / Texas A&amp;M University</t>
+          <t>University of Illinois Urbana / Southern Illinois University Carbondale</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Snidal, Duncan. “Relative Gains and the Pattern of International Cooperation.” American Political Science Review 85, no. 3 (1991): 701–26. https://doi.org/10.2307/1963847.</t>
+          <t>Mitchell, Timothy. “The Limits of the State: Beyond Statist Approaches and Their Critics.” American Political Science Review 85, no. 1 (1991): 77–96. https://doi.org/10.2307/1962879.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Many political situations involve competitions where winning is more important than doing well. In international politics, this relative gains problem is widely argued to be a major impediment to cooperation under anarchy. After discussing why states might seek relative gains, I demonstrate that the hypothesis holds very different implications from those usually presumed. Relative gains do impede cooperation in the two-actor case and provide an important justification for treating international anarchy as a prisoner's dilemma problem; but if the initial absolute gains situation is not a prisoner's dilemma, relative gains seeking is much less consequential. Its significance is even more attenuated with more than two competitors. Relative gains cannot prop up the realist critique of international cooperation theory, but may affect the pattern of cooperation when a small number of states are the most central international actors.</t>
+          <t>The state has always been difficult to define. Its boundary with
+               society appears elusive, porous, and mobile. I argue that this elusiveness should not
+               be overcome by sharper definitions, but explored as a clue to the state's nature.
+               Analysis of the literature shows that neither rejecting the state in favor of such
+               concepts as the political system, nor “bringing it back in,” has dealt with this
+               boundary problem. The former approach founders on it, the latter avoids it by a
+               narrow idealism that construes the state-society distinction as an external relation
+               between subjective and objective entities. A third approach, presented here, can
+               account for both the salience of the state and its elusiveness. Reanalyzing evidence
+               presented by recent theorists, state-society boundaries are shown to be distinctions
+               erected internally, as an aspect of more complex power relations. Their appearance
+               can be historically traced to technical innovations of the modern social order,
+               whereby methods of organization and control internal to the social processes they
+               govern create the effect of a state structure external to those
+               processes.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>University of Chicago</t>
+          <t>New York University</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
@@ -574,42 +584,185 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Remmer, Karen L. “The Political Impact of Economic Crisis in Latin America in the 1980s.” American Political Science Review 85, no. 3 (1991): 777–800. https://doi.org/10.2307/1963850.</t>
+          <t>Sinopoli, Richard C., and Nancy J. Hirschmann. “Feminism and Liberal Theory.” American Political Science Review 85, no. 1 (1991): 221–34. https://doi.org/10.2307/1962887.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Research on the political implications of economic conditions is separated into two relatively distinct bodies of literature. I bridge the theoretical gap between them by examining the effects of economic crisis on electoral outcomes in Latin America from 1982 to 1990. An analysis of 21 competitive elections indicates that crisis conditions undermine support for incumbents and provoke high levels of electoral volatility but without necessarily fostering the growth of political extremism or the exhaustion of elite consensus associated with the breakdown of democracy. The results also suggest that the relationship between economic conditions and electoral instability is mediated by party system structure rather than democratic age. Paradoxically, the findings buttress prior research on electoral outcomes in the comparatively stable and homogeneous Organization for Economic Cooperation and Development (OECD) nations while undercutting theoretical frameworks elaborated with specific reference to the breakdown and consolidation of Third World democracy.</t>
+          <t>In her article on “Freedom, Recognition, and Obligation: A Feminist Approach to Political Theory,” published in the December 1989 issue of this Review, Nancy J. Hirschmann argued that a feminist methodology could breathe new and useful life into liberal political theory, relieving it of its structural sexism. In this Controversy, Richard C. Sinopoli takes issue with key claims made by Hirschmann. In turn, Hirschmann elaborates her case.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>University of New Mexico</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
+          <t>University of California, Davis</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Cornell University</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Wood, B. Dan, and Richard W. Waterman. “The Dynamics of Political Control of the Bureaucracy.” American Political Science Review 85, no. 3 (1991): 801–28. https://doi.org/10.2307/1963851.</t>
+          <t>Baron, David P. “A Spatial Bargaining Theory of Government Formation in Parliamentary Systems.” American Political Science Review 85, no. 1 (1991): 137–64. https://doi.org/10.2307/1962882.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>A new paradigm of political-bureaucratic relations emerged through the 1980s holding that U.S. democratic institutions continuously shape nonelective public bureaucracies. Several empirical studies support the paradigm with evidence suggestive of political manipulation but none reveals the scope or specific mechanisms of political control. We explore the dynamics of political control of the bureaucracy explicitly to determine the scope and mechanisms. We examine output time series from seven different public bureaucracies for responsiveness to political tools applied in the late Carter and early Reagan administrations. We find responsiveness in all seven cases. The evidence also shows that political appointments—a shared power of the president and Congress—is the most important instrument of political control; changing budgets, legislation, congressional signals, and administrative reorganizations are less important. These findings confirm intuitive assertions by institutional scholars and suggest a method of “policy monitoring” that could enhance future democratic control of the bureaucracy.</t>
+          <t>A theory of government formation in parliamentary systems is developed from a model incorporating policy-oriented parties with spatial preferences and a formation process in which parties are selected in sequence to attempt to form a government. A government is formed when the policy proposed by the party selected is sustained on a vote of confidence. The equilibria identify the government and the policy it will implement and depend on the configuration of preferences and on the government formation process. For example, in a political system with two large parties and one small party and in which one of the two large parties will be selected to attempt to form a government, the government will be formed by a large party with the support of the small party. The policy will reflect the preferences of the small party but will be closer to the ideal point of the large party.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Texas A&amp;M University</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>University of New Mexico</t>
-        </is>
-      </c>
+          <t>Stanford University</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Epstein, Lee, and C. K. Rowland. “Debunking the Myth of Interest Group Invincibility in the Courts.” American Political Science Review 85, no. 1 (1991): 205–17. https://doi.org/10.2307/1962886.</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Research on interest group litigation has provoked a reevaluation of the conventional wisdom about the study of pressure group activity and judicial politics. Nevertheless, the notion that interest groups are intrepid litigators that rarely lose to nongroup adversaries persists unchallenged and unscathed. We seek to determine if groups are, in fact, as invincible as the literature suggests. Several findings emerge that may undermine conventional wisdom about the relative efficacy of group-sponsored litigation. Most important is that groups are no more likely than nongroups to win, at least in U.S. District Courts. Based on this and other results, we draw a number of conclusions about interest group litigation and the direction into which future study might head.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Southern Methodist University</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>University of Kansas</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Goldstein, Joshua S., and John R. Freeman. “U.S.-Soviet-Chinese Relations: Routine, Reciprocity, or Rational Expectations?” American Political Science Review 85, no. 1 (1991): 17–35. https://doi.org/10.2307/1962876.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>International relations theorists disagree about whether great power behaviors reflect bureaucratic routine or reciprocity. Recently, some have suggested that these behaviors result from great powers' rational expectations rather than from simple routine or reciprocity. The debate is flawed in several respects. The quasi-experimental studies of great power behavior suffer from specification and measurement errors. Furthermore, most studies of great power behavior focus exclusively on the superpowers, without adequately appreciating China's role in world politics. We present an improved analysis that recognizes the potential effects of Chinese behavior and ameliorates the methodological flaws in existing work. The results indicate that the behaviors of the United States, the Soviet Union, and China are a relatively stable mix of bureaucratic routine and reciprocity. The results also indicate complex, asymmetrical connections among U.S.-Soviet, U.S.-Chinese, and Soviet-Chinese relations, consistent with the notion of a strategic triangle.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>University of Southern California</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>University of Minnesota</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Shklar, Judith N. “Redeeming American Political Theory.” American Political Science Review 85, no. 1 (1991): 3–15. https://doi.org/10.2307/1962875.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>American political theory has been accused of being uniformly liberal; but its history is diverse and is worth studying to understand the development of political science and the institutions it reflects (representative government, federalism, judicial review, and slavery). While modern social science expresses a slow democratization of values, it has been compatible with many ideologies. This can be seen in Jefferson's anthropology, Madison's theory of collective rationality, and Hamilton's empirical political economy. Jacksonian democracy encouraged social history, while its opponents devised an elitist political sociology. Southern defenders of slavery were the earliest to develop a deterministic and authoritarian sociology, but after the Civil War Northern thinkers emulated them with Social Darwinism and quests for causal laws to grasp constant change in industrial society. Though social critics abounded, democratic empirical theory emerged in the universities only in the generation of Merriam and Dewey, who founded contemporary political science.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Harvard University</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Honig, B. “Declarations of Independence: Arendt and Derrida on the Problem of Founding a Republic.” American Political Science Review 85, no. 1 (1991): 97–113. https://doi.org/10.2307/1962880.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Beginning with Hannah Arendt's depiction of the American Revolution and founding, I critically examine Arendt's reading of the Declaration of Independence, comparing it with Jacques Derrida's reading of (a draft of) the same document, in order to show that Arendt is careless in her easy dismissal of the declaration's essentialist moments. Derrida, it seems to me, has a better, more subtle appreciation of the both necessary and impossible role of essentialism in modern political theory and practice. I conclude, however, that Arendt nonetheless succeeds in theorizing a powerful and suggestive practice of political authority for modernity, a practice that is uniquely activist and appropriate for a democratic politics.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Harvard University</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ostrom, Elinor. “Rational Choice Theory and Institutional Analysis: Toward Complementarity.” American Political Science Review 85, no. 1 (1991): 237–43. https://doi.org/10.2307/1962888.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Indiana University</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Schonhardt-Bailey, Cheryl. “Lessons in Lobbying for Free Trade in 19th-Century Britain: To Concentrate or Not.” American Political Science Review 85, no. 1 (1991): 37–58. https://doi.org/10.2307/1962877.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>I present a modified version of the public choice interest group model that integrates concentrated and deconcentrated interests with successful lobbying. It is argued that effective free trade lobbying required the political fusion of the economic interests representing two fundamental changes in nineteenth-century Britain's economy: (1) geographic concentration of the core export industry (cotton textiles) and (2) deconcentration of the broader export sector both geographically and in terms of industrial structure. Empirical evidence from both national and individual levels firmly supports the contention that the timing and political success of Britain's nineteenth-century free trade lobby required the combined forces of core export interests and the more diverse and geographically more evenly distributed interests of the export sector as a whole.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>University of California Los Angeles London School of Economics and Political Science</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Booth, William James. “The New Household Economy.” American Political Science Review 85, no. 1 (1991): 59–75. https://doi.org/10.2307/1962878.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>In the revival of scholarly interest in Marx's relationship to one of the greatest of
+his teachers, Aristotle, a crucial aspect has been undervalued: Marx's indebtedness
+to ancient political economy. While Marx employed the methods and key concepts of the
+economic science of his day in analyzing capitalism, he embedded that explanation in
+a higher-order theory of the economy. This theory, derived from the Aristotelian
+account of the household economy, seeks to situate the economy in an overarching
+account of the community, its purposiveness, and the place within it of activity,
+time, and domination. Marx sought thereby to illuminate the historical uniqueness of
+capitalism and, relatedly, to show the bounded character of the economic science
+(including his own) appropriate to the understanding of it. Central elements of the
+Aristotelian critique of an economy given over to Midas-like acquisition also find
+their way into Marx's evaluation of capitalism, and the ideal of the ancient
+oikos forms one of the core parts of Marx's theory of communism
+as the new household economy.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>McGill University</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>